<commit_message>
update data to 8/23
</commit_message>
<xml_diff>
--- a/data/FNs catch 2024.xlsx
+++ b/data/FNs catch 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{91671601-6ECB-0D46-B14E-AB8D1443C034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{905C686D-9BE7-4CA5-A69F-1D588D15DB5A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AF67EE-4CFA-DC4C-B166-7594A5B55DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="710" yWindow="660" windowWidth="11410" windowHeight="12210" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
+    <workbookView xWindow="16360" yWindow="500" windowWidth="20920" windowHeight="15900" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sockeye FSC and Demo" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>In-River Skeena FSC Catch Numbers - DO NOT SHARE BEYOND SFNTC</t>
   </si>
@@ -220,10 +220,10 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1552,12 +1552,12 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2023</v>
       </c>
@@ -1579,19 +1579,19 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
       <c r="T3" t="s">
         <v>2</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>24</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>25</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>26</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>28</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>29</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>31</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>32</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="F13" s="2">
         <v>394</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>4000</v>
       </c>
       <c r="H13" s="2">
@@ -2207,7 +2207,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>33</v>
       </c>
@@ -2220,7 +2220,9 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>2548</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="L14">
@@ -2237,7 +2239,7 @@
       </c>
       <c r="O14">
         <f t="shared" si="1"/>
-        <v>8813</v>
+        <v>11361</v>
       </c>
       <c r="P14">
         <f t="shared" si="1"/>
@@ -2264,7 +2266,7 @@
         <v>48135</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>34</v>
       </c>
@@ -2294,7 +2296,7 @@
       </c>
       <c r="O15">
         <f t="shared" si="1"/>
-        <v>8813</v>
+        <v>11361</v>
       </c>
       <c r="P15">
         <f t="shared" si="1"/>
@@ -2314,14 +2316,14 @@
       </c>
       <c r="U15">
         <f t="shared" si="5"/>
-        <v>42135</v>
+        <v>44683</v>
       </c>
       <c r="V15">
         <f t="shared" si="3"/>
-        <v>48529</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
+        <v>51077</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>35</v>
       </c>
@@ -2351,7 +2353,7 @@
       </c>
       <c r="O16">
         <f t="shared" si="1"/>
-        <v>8813</v>
+        <v>11361</v>
       </c>
       <c r="P16">
         <f t="shared" si="1"/>
@@ -2371,14 +2373,14 @@
       </c>
       <c r="U16">
         <f t="shared" si="5"/>
-        <v>42135</v>
+        <v>44683</v>
       </c>
       <c r="V16">
         <f t="shared" si="3"/>
-        <v>48529</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
+        <v>51077</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>36</v>
       </c>
@@ -2408,7 +2410,7 @@
       </c>
       <c r="O17">
         <f t="shared" si="1"/>
-        <v>8813</v>
+        <v>11361</v>
       </c>
       <c r="P17">
         <f t="shared" si="1"/>
@@ -2428,14 +2430,14 @@
       </c>
       <c r="U17">
         <f t="shared" si="5"/>
-        <v>42135</v>
+        <v>44683</v>
       </c>
       <c r="V17">
         <f t="shared" si="3"/>
-        <v>48529</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
+        <v>51077</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C18" s="9" t="s">
         <v>17</v>
       </c>
@@ -2453,7 +2455,7 @@
       </c>
       <c r="H18" s="2">
         <f t="shared" si="6"/>
-        <v>8813</v>
+        <v>11361</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="6"/>
@@ -2480,9 +2482,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2493,7 +2495,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>45452</v>
       </c>
@@ -2506,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>45453</v>
       </c>
@@ -2519,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>45454</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>45455</v>
       </c>
@@ -2545,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>45456</v>
       </c>
@@ -2558,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>45457</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>45458</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>45459</v>
       </c>
@@ -2597,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>45460</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>45461</v>
       </c>
@@ -2623,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>45462</v>
       </c>
@@ -2636,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>45463</v>
       </c>
@@ -2649,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>45464</v>
       </c>
@@ -2662,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>45465</v>
       </c>
@@ -2675,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>45466</v>
       </c>
@@ -2688,7 +2690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>45467</v>
       </c>
@@ -2701,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>45468</v>
       </c>
@@ -2714,7 +2716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>45469</v>
       </c>
@@ -2727,7 +2729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>45470</v>
       </c>
@@ -2740,7 +2742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>45471</v>
       </c>
@@ -2753,7 +2755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>45472</v>
       </c>
@@ -2766,7 +2768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>45473</v>
       </c>
@@ -2779,7 +2781,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>45474</v>
       </c>
@@ -2792,7 +2794,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>45475</v>
       </c>
@@ -2805,7 +2807,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>45476</v>
       </c>
@@ -2818,7 +2820,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>45477</v>
       </c>
@@ -2831,7 +2833,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>45478</v>
       </c>
@@ -2844,7 +2846,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>45479</v>
       </c>
@@ -2857,7 +2859,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>45480</v>
       </c>
@@ -2870,7 +2872,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>45481</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>45482</v>
       </c>
@@ -2896,7 +2898,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>45483</v>
       </c>
@@ -2909,7 +2911,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>45484</v>
       </c>
@@ -2922,7 +2924,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>45485</v>
       </c>
@@ -2935,7 +2937,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>45486</v>
       </c>
@@ -2948,7 +2950,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>45487</v>
       </c>
@@ -2961,7 +2963,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>45488</v>
       </c>
@@ -2974,7 +2976,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>45489</v>
       </c>
@@ -2987,7 +2989,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>45490</v>
       </c>
@@ -3000,7 +3002,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>45491</v>
       </c>
@@ -3013,7 +3015,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>45492</v>
       </c>
@@ -3026,7 +3028,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>45493</v>
       </c>
@@ -3039,7 +3041,7 @@
         <v>6304</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>45494</v>
       </c>
@@ -3052,7 +3054,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>45495</v>
       </c>
@@ -3065,7 +3067,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>45496</v>
       </c>
@@ -3078,7 +3080,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>45497</v>
       </c>
@@ -3091,7 +3093,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>45498</v>
       </c>
@@ -3104,7 +3106,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>45499</v>
       </c>
@@ -3117,7 +3119,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>45500</v>
       </c>
@@ -3130,7 +3132,7 @@
         <v>14368</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>45501</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>45502</v>
       </c>
@@ -3156,7 +3158,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>45503</v>
       </c>
@@ -3169,7 +3171,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>45504</v>
       </c>
@@ -3182,7 +3184,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
         <v>45505</v>
       </c>
@@ -3195,7 +3197,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>45506</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>45507</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>23285</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>45508</v>
       </c>
@@ -3234,7 +3236,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>45509</v>
       </c>
@@ -3247,7 +3249,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>45510</v>
       </c>
@@ -3260,7 +3262,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>45511</v>
       </c>
@@ -3273,7 +3275,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>45512</v>
       </c>
@@ -3286,7 +3288,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>45513</v>
       </c>
@@ -3299,7 +3301,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
         <v>45514</v>
       </c>
@@ -3312,7 +3314,7 @@
         <v>32815</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>45515</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>48135</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>45516</v>
       </c>
@@ -3338,7 +3340,7 @@
         <v>48135</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>45517</v>
       </c>
@@ -3351,7 +3353,7 @@
         <v>48135</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
         <v>45518</v>
       </c>
@@ -3364,7 +3366,7 @@
         <v>48135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
         <v>45519</v>
       </c>
@@ -3374,7 +3376,7 @@
       </c>
       <c r="C69" s="10"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
         <v>45520</v>
       </c>
@@ -3384,7 +3386,7 @@
       </c>
       <c r="C70" s="10"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="11">
         <v>45521</v>
       </c>
@@ -3394,7 +3396,7 @@
       </c>
       <c r="C71" s="10"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>45522</v>
       </c>
@@ -3404,7 +3406,7 @@
       </c>
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>45523</v>
       </c>
@@ -3414,7 +3416,7 @@
       </c>
       <c r="C73" s="10"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>45524</v>
       </c>
@@ -3424,7 +3426,7 @@
       </c>
       <c r="C74" s="10"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>45525</v>
       </c>
@@ -3434,7 +3436,7 @@
       </c>
       <c r="C75" s="10"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>45526</v>
       </c>
@@ -3444,7 +3446,7 @@
       </c>
       <c r="C76" s="10"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
         <v>45527</v>
       </c>
@@ -3454,7 +3456,7 @@
       </c>
       <c r="C77" s="10"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
         <v>45528</v>
       </c>
@@ -3464,7 +3466,7 @@
       </c>
       <c r="C78" s="10"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="11">
         <v>45529</v>
       </c>
@@ -3474,7 +3476,7 @@
       </c>
       <c r="C79" s="10"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
         <v>45530</v>
       </c>
@@ -3484,7 +3486,7 @@
       </c>
       <c r="C80" s="10"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
         <v>45531</v>
       </c>
@@ -3494,7 +3496,7 @@
       </c>
       <c r="C81" s="10"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
         <v>45532</v>
       </c>
@@ -3504,7 +3506,7 @@
       </c>
       <c r="C82" s="10"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
         <v>45533</v>
       </c>
@@ -3514,7 +3516,7 @@
       </c>
       <c r="C83" s="10"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
         <v>45534</v>
       </c>
@@ -3524,7 +3526,7 @@
       </c>
       <c r="C84" s="10"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
         <v>45535</v>
       </c>
@@ -3534,7 +3536,7 @@
       </c>
       <c r="C85" s="10"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
         <v>45536</v>
       </c>
@@ -3544,7 +3546,7 @@
       </c>
       <c r="C86" s="10"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
         <v>45537</v>
       </c>
@@ -3554,7 +3556,7 @@
       </c>
       <c r="C87" s="10"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="11">
         <v>45538</v>
       </c>
@@ -3564,7 +3566,7 @@
       </c>
       <c r="C88" s="10"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
         <v>45539</v>
       </c>
@@ -3574,7 +3576,7 @@
       </c>
       <c r="C89" s="10"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="11">
         <v>45540</v>
       </c>
@@ -3584,7 +3586,7 @@
       </c>
       <c r="C90" s="10"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
         <v>45541</v>
       </c>
@@ -3594,7 +3596,7 @@
       </c>
       <c r="C91" s="10"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="11">
         <v>45542</v>
       </c>
@@ -3611,15 +3613,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A7F00F-86F9-7B42-9119-B394F847541D}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3639,7 +3641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>45490</v>
       </c>
@@ -3653,7 +3655,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>45490</v>
       </c>
@@ -3667,7 +3669,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>45497</v>
       </c>
@@ -3681,7 +3683,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>45501</v>
       </c>
@@ -3695,7 +3697,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>45501</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>45505</v>
       </c>
@@ -3723,7 +3725,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>45506</v>
       </c>
@@ -3737,7 +3739,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>45506</v>
       </c>
@@ -3751,7 +3753,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>45508</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>45509</v>
       </c>
@@ -3779,7 +3781,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>45509</v>
       </c>
@@ -3793,7 +3795,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>45510</v>
       </c>
@@ -3807,7 +3809,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>45510</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>45510</v>
       </c>
@@ -3835,7 +3837,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>45511</v>
       </c>
@@ -3849,7 +3851,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>45511</v>
       </c>
@@ -3863,7 +3865,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>45512</v>
       </c>
@@ -3877,7 +3879,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>45513</v>
       </c>
@@ -3891,7 +3893,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>45514</v>
       </c>
@@ -3905,7 +3907,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>45515</v>
       </c>
@@ -3919,7 +3921,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>45515</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>45516</v>
       </c>
@@ -3945,6 +3947,104 @@
       </c>
       <c r="D23">
         <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
+        <v>45517</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>45518</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>45519</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
+        <v>45520</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>45521</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <v>45522</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>45523</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8/30 update Tyee data and fisheries openings
</commit_message>
<xml_diff>
--- a/data/FNs catch 2024.xlsx
+++ b/data/FNs catch 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AF67EE-4CFA-DC4C-B166-7594A5B55DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD5A62D-1B28-C14F-B62F-7014722F8E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16360" yWindow="500" windowWidth="20920" windowHeight="15900" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
+    <workbookView xWindow="13320" yWindow="500" windowWidth="20920" windowHeight="15900" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sockeye FSC and Demo" sheetId="1" r:id="rId1"/>
@@ -1551,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F517E49F-3167-EC43-A232-0380675D9406}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1672,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="N5">
         <f>G5</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <f>H5</f>
@@ -1729,9 +1729,11 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
       <c r="G6" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1743,11 +1745,11 @@
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
@@ -1787,9 +1789,11 @@
         <v>45472</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>79</v>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1800,11 +1804,11 @@
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
@@ -1828,11 +1832,11 @@
       </c>
       <c r="U7">
         <f t="shared" ref="U7:U17" si="5">SUM(N6+O6)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="V7">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -1846,9 +1850,11 @@
         <v>45479</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="7">
-        <v>2332</v>
+      <c r="F8" s="2">
+        <v>248</v>
+      </c>
+      <c r="G8" s="2">
+        <v>79</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="2"/>
@@ -1859,11 +1865,11 @@
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>263</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>2418</v>
+        <v>86</v>
       </c>
       <c r="O8">
         <f t="shared" si="1"/>
@@ -1883,15 +1889,15 @@
       </c>
       <c r="T8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U8">
         <f t="shared" si="5"/>
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="V8">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
@@ -1905,9 +1911,12 @@
         <v>45486</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <f>80+68+118+36+173+112+127</f>
+        <v>714</v>
+      </c>
       <c r="G9" s="7">
-        <v>3886</v>
+        <v>2332</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="2"/>
@@ -1918,11 +1927,11 @@
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>977</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>6304</v>
+        <v>2418</v>
       </c>
       <c r="O9">
         <f t="shared" si="1"/>
@@ -1942,15 +1951,15 @@
       </c>
       <c r="T9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U9">
         <f t="shared" si="5"/>
-        <v>2418</v>
+        <v>86</v>
       </c>
       <c r="V9">
         <f t="shared" si="3"/>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -1967,10 +1976,10 @@
         <v>100</v>
       </c>
       <c r="F10" s="2">
-        <v>100</v>
+        <v>636</v>
       </c>
       <c r="G10" s="7">
-        <v>8064</v>
+        <v>3886</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="2"/>
@@ -1981,11 +1990,11 @@
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>1613</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
-        <v>14368</v>
+        <v>6304</v>
       </c>
       <c r="O10">
         <f t="shared" si="1"/>
@@ -2005,15 +2014,15 @@
       </c>
       <c r="T10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>263</v>
       </c>
       <c r="U10">
         <f t="shared" si="5"/>
-        <v>6304</v>
+        <v>2418</v>
       </c>
       <c r="V10">
         <f t="shared" si="3"/>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -2030,10 +2039,10 @@
         <v>900</v>
       </c>
       <c r="F11" s="2">
-        <v>900</v>
-      </c>
-      <c r="G11" s="2">
-        <v>8717</v>
+        <v>661</v>
+      </c>
+      <c r="G11" s="7">
+        <v>8064</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2044,11 +2053,11 @@
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2274</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>23085</v>
+        <v>14368</v>
       </c>
       <c r="O11">
         <f t="shared" si="1"/>
@@ -2068,15 +2077,15 @@
       </c>
       <c r="T11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>977</v>
       </c>
       <c r="U11">
         <f t="shared" si="5"/>
-        <v>14368</v>
+        <v>6304</v>
       </c>
       <c r="V11">
         <f t="shared" si="3"/>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -2093,10 +2102,10 @@
         <v>2000</v>
       </c>
       <c r="F12" s="2">
-        <v>2000</v>
+        <v>491</v>
       </c>
       <c r="G12" s="2">
-        <v>6237</v>
+        <v>8717</v>
       </c>
       <c r="H12" s="2">
         <v>1493</v>
@@ -2109,11 +2118,11 @@
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2765</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
-        <v>29322</v>
+        <v>23085</v>
       </c>
       <c r="O12">
         <f t="shared" si="1"/>
@@ -2133,15 +2142,15 @@
       </c>
       <c r="T12">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>1713</v>
       </c>
       <c r="U12">
         <f t="shared" si="5"/>
-        <v>23085</v>
+        <v>14368</v>
       </c>
       <c r="V12">
         <f t="shared" si="3"/>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -2156,10 +2165,10 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="G13" s="12">
-        <v>4000</v>
+        <v>7946</v>
       </c>
       <c r="H13" s="2">
         <v>7320</v>
@@ -2172,11 +2181,11 @@
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>3394</v>
+        <v>3141</v>
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
-        <v>33322</v>
+        <v>31031</v>
       </c>
       <c r="O13">
         <f t="shared" si="1"/>
@@ -2196,15 +2205,15 @@
       </c>
       <c r="T13">
         <f t="shared" si="4"/>
-        <v>2000</v>
+        <v>3274</v>
       </c>
       <c r="U13">
         <f t="shared" si="5"/>
-        <v>30815</v>
+        <v>24578</v>
       </c>
       <c r="V13">
         <f t="shared" si="3"/>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -2218,8 +2227,12 @@
         <v>45521</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2">
+        <v>376</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3025</v>
+      </c>
       <c r="H14" s="2">
         <v>2548</v>
       </c>
@@ -2231,11 +2244,11 @@
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>3394</v>
+        <v>3517</v>
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>33322</v>
+        <v>34056</v>
       </c>
       <c r="O14">
         <f t="shared" si="1"/>
@@ -2255,15 +2268,15 @@
       </c>
       <c r="T14">
         <f t="shared" si="4"/>
-        <v>6000</v>
+        <v>5765</v>
       </c>
       <c r="U14">
         <f t="shared" si="5"/>
-        <v>42135</v>
+        <v>39844</v>
       </c>
       <c r="V14">
         <f t="shared" si="3"/>
-        <v>48135</v>
+        <v>45609</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -2277,8 +2290,12 @@
         <v>45528</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="2">
+        <v>90</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2779</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2288,11 +2305,11 @@
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>3394</v>
+        <v>3607</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>33322</v>
+        <v>36835</v>
       </c>
       <c r="O15">
         <f t="shared" si="1"/>
@@ -2312,15 +2329,15 @@
       </c>
       <c r="T15">
         <f t="shared" si="4"/>
-        <v>6394</v>
+        <v>6141</v>
       </c>
       <c r="U15">
         <f t="shared" si="5"/>
-        <v>44683</v>
+        <v>45417</v>
       </c>
       <c r="V15">
         <f t="shared" si="3"/>
-        <v>51077</v>
+        <v>51558</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -2335,7 +2352,9 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2345,11 +2364,11 @@
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>3394</v>
+        <v>3607</v>
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
-        <v>33322</v>
+        <v>36835</v>
       </c>
       <c r="O16">
         <f t="shared" si="1"/>
@@ -2369,15 +2388,15 @@
       </c>
       <c r="T16">
         <f t="shared" si="4"/>
-        <v>6394</v>
+        <v>6517</v>
       </c>
       <c r="U16">
         <f t="shared" si="5"/>
-        <v>44683</v>
+        <v>48196</v>
       </c>
       <c r="V16">
         <f t="shared" si="3"/>
-        <v>51077</v>
+        <v>54713</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -2402,11 +2421,11 @@
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>3394</v>
+        <v>3607</v>
       </c>
       <c r="N17">
         <f t="shared" si="1"/>
-        <v>33322</v>
+        <v>36835</v>
       </c>
       <c r="O17">
         <f t="shared" si="1"/>
@@ -2426,15 +2445,15 @@
       </c>
       <c r="T17">
         <f t="shared" si="4"/>
-        <v>6394</v>
+        <v>6607</v>
       </c>
       <c r="U17">
         <f t="shared" si="5"/>
-        <v>44683</v>
+        <v>48196</v>
       </c>
       <c r="V17">
         <f t="shared" si="3"/>
-        <v>51077</v>
+        <v>54803</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -2446,12 +2465,12 @@
         <v>3000</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="6"/>
-        <v>3394</v>
+        <f>SUM(F6:F17)</f>
+        <v>3607</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="6"/>
-        <v>33315</v>
+        <v>36831</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="6"/>
@@ -2478,8 +2497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D5C568-A1B0-4A43-9C92-FB0E4EE097B2}">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2687,7 +2706,7 @@
       </c>
       <c r="C16" s="10">
         <f>VLOOKUP('inriver catch'!B16,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2700,7 +2719,7 @@
       </c>
       <c r="C17" s="10">
         <f>VLOOKUP('inriver catch'!B17,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2713,7 +2732,7 @@
       </c>
       <c r="C18" s="10">
         <f>VLOOKUP('inriver catch'!B18,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2726,7 +2745,7 @@
       </c>
       <c r="C19" s="10">
         <f>VLOOKUP('inriver catch'!B19,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2739,7 +2758,7 @@
       </c>
       <c r="C20" s="10">
         <f>VLOOKUP('inriver catch'!B20,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2752,7 +2771,7 @@
       </c>
       <c r="C21" s="10">
         <f>VLOOKUP('inriver catch'!B21,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2765,7 +2784,7 @@
       </c>
       <c r="C22" s="10">
         <f>VLOOKUP('inriver catch'!B22,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2778,7 +2797,7 @@
       </c>
       <c r="C23" s="10">
         <f>VLOOKUP('inriver catch'!B23,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2791,7 +2810,7 @@
       </c>
       <c r="C24" s="10">
         <f>VLOOKUP('inriver catch'!B24,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2804,7 +2823,7 @@
       </c>
       <c r="C25" s="10">
         <f>VLOOKUP('inriver catch'!B25,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2817,7 +2836,7 @@
       </c>
       <c r="C26" s="10">
         <f>VLOOKUP('inriver catch'!B26,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2830,7 +2849,7 @@
       </c>
       <c r="C27" s="10">
         <f>VLOOKUP('inriver catch'!B27,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2843,7 +2862,7 @@
       </c>
       <c r="C28" s="10">
         <f>VLOOKUP('inriver catch'!B28,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2856,7 +2875,7 @@
       </c>
       <c r="C29" s="10">
         <f>VLOOKUP('inriver catch'!B29,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2869,7 +2888,7 @@
       </c>
       <c r="C30" s="10">
         <f>VLOOKUP('inriver catch'!B30,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2882,7 +2901,7 @@
       </c>
       <c r="C31" s="10">
         <f>VLOOKUP('inriver catch'!B31,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2895,7 +2914,7 @@
       </c>
       <c r="C32" s="10">
         <f>VLOOKUP('inriver catch'!B32,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2908,7 +2927,7 @@
       </c>
       <c r="C33" s="10">
         <f>VLOOKUP('inriver catch'!B33,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2921,7 +2940,7 @@
       </c>
       <c r="C34" s="10">
         <f>VLOOKUP('inriver catch'!B34,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2934,7 +2953,7 @@
       </c>
       <c r="C35" s="10">
         <f>VLOOKUP('inriver catch'!B35,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2947,7 +2966,7 @@
       </c>
       <c r="C36" s="10">
         <f>VLOOKUP('inriver catch'!B36,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2418</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2960,7 +2979,7 @@
       </c>
       <c r="C37" s="10">
         <f>VLOOKUP('inriver catch'!B37,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2973,7 +2992,7 @@
       </c>
       <c r="C38" s="10">
         <f>VLOOKUP('inriver catch'!B38,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2986,7 +3005,7 @@
       </c>
       <c r="C39" s="10">
         <f>VLOOKUP('inriver catch'!B39,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2999,7 +3018,7 @@
       </c>
       <c r="C40" s="10">
         <f>VLOOKUP('inriver catch'!B40,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3012,7 +3031,7 @@
       </c>
       <c r="C41" s="10">
         <f>VLOOKUP('inriver catch'!B41,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3025,7 +3044,7 @@
       </c>
       <c r="C42" s="10">
         <f>VLOOKUP('inriver catch'!B42,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3038,7 +3057,7 @@
       </c>
       <c r="C43" s="10">
         <f>VLOOKUP('inriver catch'!B43,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>6304</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3051,7 +3070,7 @@
       </c>
       <c r="C44" s="10">
         <f>VLOOKUP('inriver catch'!B44,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -3064,7 +3083,7 @@
       </c>
       <c r="C45" s="10">
         <f>VLOOKUP('inriver catch'!B45,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -3077,7 +3096,7 @@
       </c>
       <c r="C46" s="10">
         <f>VLOOKUP('inriver catch'!B46,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3090,7 +3109,7 @@
       </c>
       <c r="C47" s="10">
         <f>VLOOKUP('inriver catch'!B47,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -3103,7 +3122,7 @@
       </c>
       <c r="C48" s="10">
         <f>VLOOKUP('inriver catch'!B48,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3116,7 +3135,7 @@
       </c>
       <c r="C49" s="10">
         <f>VLOOKUP('inriver catch'!B49,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3129,7 +3148,7 @@
       </c>
       <c r="C50" s="10">
         <f>VLOOKUP('inriver catch'!B50,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>14368</v>
+        <v>7281</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3142,7 +3161,7 @@
       </c>
       <c r="C51" s="10">
         <f>VLOOKUP('inriver catch'!B51,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3155,7 +3174,7 @@
       </c>
       <c r="C52" s="10">
         <f>VLOOKUP('inriver catch'!B52,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3168,7 +3187,7 @@
       </c>
       <c r="C53" s="10">
         <f>VLOOKUP('inriver catch'!B53,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3181,7 +3200,7 @@
       </c>
       <c r="C54" s="10">
         <f>VLOOKUP('inriver catch'!B54,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3194,7 +3213,7 @@
       </c>
       <c r="C55" s="10">
         <f>VLOOKUP('inriver catch'!B55,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3207,7 +3226,7 @@
       </c>
       <c r="C56" s="10">
         <f>VLOOKUP('inriver catch'!B56,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3220,7 +3239,7 @@
       </c>
       <c r="C57" s="10">
         <f>VLOOKUP('inriver catch'!B57,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>23285</v>
+        <v>16081</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3233,7 +3252,7 @@
       </c>
       <c r="C58" s="10">
         <f>VLOOKUP('inriver catch'!B58,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3246,7 +3265,7 @@
       </c>
       <c r="C59" s="10">
         <f>VLOOKUP('inriver catch'!B59,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3259,7 +3278,7 @@
       </c>
       <c r="C60" s="10">
         <f>VLOOKUP('inriver catch'!B60,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3272,7 +3291,7 @@
       </c>
       <c r="C61" s="10">
         <f>VLOOKUP('inriver catch'!B61,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3285,7 +3304,7 @@
       </c>
       <c r="C62" s="10">
         <f>VLOOKUP('inriver catch'!B62,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3298,7 +3317,7 @@
       </c>
       <c r="C63" s="10">
         <f>VLOOKUP('inriver catch'!B63,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -3311,7 +3330,7 @@
       </c>
       <c r="C64" s="10">
         <f>VLOOKUP('inriver catch'!B64,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>32815</v>
+        <v>27852</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -3324,7 +3343,7 @@
       </c>
       <c r="C65" s="10">
         <f>VLOOKUP('inriver catch'!B65,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>48135</v>
+        <v>45609</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -3337,7 +3356,7 @@
       </c>
       <c r="C66" s="10">
         <f>VLOOKUP('inriver catch'!B66,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>48135</v>
+        <v>45609</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -3350,7 +3369,7 @@
       </c>
       <c r="C67" s="10">
         <f>VLOOKUP('inriver catch'!B67,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>48135</v>
+        <v>45609</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -3363,7 +3382,7 @@
       </c>
       <c r="C68" s="10">
         <f>VLOOKUP('inriver catch'!B68,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>48135</v>
+        <v>45609</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -3615,7 +3634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A7F00F-86F9-7B42-9119-B394F847541D}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update demo catches with Metlakatla data
</commit_message>
<xml_diff>
--- a/data/FNs catch 2024.xlsx
+++ b/data/FNs catch 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{29AF67EE-4CFA-DC4C-B166-7594A5B55DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B6DA0A9-514F-4497-AEC3-32240E0D0324}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773DDB40-28A5-8647-B660-428C85447036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3190" yWindow="2190" windowWidth="16270" windowHeight="11900" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
+    <workbookView xWindow="10240" yWindow="500" windowWidth="27820" windowHeight="17500" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sockeye FSC and Demo" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
   <si>
     <t>In-River Skeena FSC Catch Numbers - DO NOT SHARE BEYOND SFNTC</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Beach seine</t>
+  </si>
+  <si>
+    <t>Metlakatla</t>
   </si>
 </sst>
 </file>
@@ -1549,15 +1552,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F517E49F-3167-EC43-A232-0380675D9406}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1567,8 +1570,9 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2023</v>
       </c>
@@ -1578,8 +1582,9 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1592,14 +1597,15 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
-      <c r="T3" t="s">
+      <c r="K3" s="13"/>
+      <c r="U3" t="s">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="29.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1628,37 +1634,40 @@
       <c r="J4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="4" t="s">
+      <c r="K4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="4"/>
+      <c r="T4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>24</v>
       </c>
@@ -1677,47 +1686,48 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5">
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="M5">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f>F5</f>
         <v>0</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f>G5</f>
         <v>4</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f>H5</f>
         <v>0</v>
       </c>
-      <c r="P5">
-        <f t="shared" ref="P5" si="0">I5</f>
-        <v>0</v>
-      </c>
       <c r="Q5">
+        <f t="shared" ref="Q5" si="0">I5</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
         <f>J5</f>
         <v>0</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <f>A5</f>
         <v>24</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
-        <f>SUM(T5:U5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>SUM(U5:V5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>25</v>
       </c>
@@ -1736,47 +1746,48 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
-      <c r="L6">
-        <f t="shared" ref="L6:Q17" si="1">L5+E6</f>
-        <v>0</v>
-      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
       <c r="M6">
-        <f t="shared" si="1"/>
+        <f>M5+E6</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
+        <f>N5+F6</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>O5+G6</f>
         <v>7</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P6">
-        <f t="shared" si="1"/>
+        <f>P5+H6</f>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <f t="shared" ref="S6:S17" si="2">A6</f>
+        <f>Q5+I6</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f>R5+J6</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6:T17" si="1">A6</f>
         <v>25</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" ref="V6:V17" si="3">SUM(T6:U6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ref="W6:W17" si="2">SUM(U6:V6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>26</v>
       </c>
@@ -1794,48 +1805,49 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="L7">
+      <c r="K7" s="2"/>
+      <c r="M7">
+        <f>M6+E7</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>N6+F7</f>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>O6+G7</f>
+        <v>86</v>
+      </c>
+      <c r="P7">
+        <f>P6+H7</f>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>Q6+I7</f>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f>R6+J7</f>
+        <v>0</v>
+      </c>
+      <c r="T7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S7">
+        <v>26</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U17" si="3">SUM(M5+N5)</f>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f t="shared" ref="V7:V17" si="4">SUM(O6+P6)</f>
+        <v>7</v>
+      </c>
+      <c r="W7">
         <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="T7">
-        <f t="shared" ref="T7:T17" si="4">SUM(L5+M5)</f>
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <f t="shared" ref="U7:U17" si="5">SUM(N6+O6)</f>
         <v>7</v>
       </c>
-      <c r="V7">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
@@ -1853,48 +1865,49 @@
       <c r="H8" s="8"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="L8">
+      <c r="K8" s="2"/>
+      <c r="M8">
+        <f>M7+E8</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>N7+F8</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>O7+G8</f>
+        <v>2418</v>
+      </c>
+      <c r="P8">
+        <f>P7+H8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f>Q7+I8</f>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f>R7+J8</f>
+        <v>0</v>
+      </c>
+      <c r="T8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="1"/>
-        <v>2418</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S8">
+        <v>27</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="5"/>
         <v>86</v>
       </c>
-      <c r="V8">
-        <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>28</v>
       </c>
@@ -1912,48 +1925,49 @@
       <c r="H9" s="8"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="L9">
+      <c r="K9" s="2"/>
+      <c r="M9">
+        <f>M8+E9</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>N8+F9</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>O8+G9</f>
+        <v>6304</v>
+      </c>
+      <c r="P9">
+        <f>P8+H9</f>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f>Q8+I9</f>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f>R8+J9</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="1"/>
-        <v>6304</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S9">
+        <v>28</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="4"/>
+        <v>2418</v>
+      </c>
+      <c r="W9">
         <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="5"/>
         <v>2418</v>
       </c>
-      <c r="V9">
-        <f t="shared" si="3"/>
-        <v>2418</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>29</v>
       </c>
@@ -1975,48 +1989,49 @@
       <c r="H10" s="8"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="L10">
+      <c r="K10" s="2"/>
+      <c r="M10">
+        <f>M9+E10</f>
+        <v>100</v>
+      </c>
+      <c r="N10">
+        <f>N9+F10</f>
+        <v>100</v>
+      </c>
+      <c r="O10">
+        <f>O9+G10</f>
+        <v>14368</v>
+      </c>
+      <c r="P10">
+        <f>P9+H10</f>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f>Q9+I10</f>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f>R9+J10</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
         <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="1"/>
-        <v>14368</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S10">
+        <v>29</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="4"/>
+        <v>6304</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="5"/>
         <v>6304</v>
       </c>
-      <c r="V10">
-        <f t="shared" si="3"/>
-        <v>6304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30</v>
       </c>
@@ -2038,48 +2053,49 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="L11">
+      <c r="K11" s="2"/>
+      <c r="M11">
+        <f>M10+E11</f>
+        <v>1000</v>
+      </c>
+      <c r="N11">
+        <f>N10+F11</f>
+        <v>1000</v>
+      </c>
+      <c r="O11">
+        <f>O10+G11</f>
+        <v>23085</v>
+      </c>
+      <c r="P11">
+        <f>P10+H11</f>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f>Q10+I11</f>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f>R10+J11</f>
+        <v>0</v>
+      </c>
+      <c r="T11">
         <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="1"/>
-        <v>23085</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S11">
+        <v>30</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="4"/>
+        <v>14368</v>
+      </c>
+      <c r="W11">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="5"/>
         <v>14368</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="3"/>
-        <v>14368</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>31</v>
       </c>
@@ -2103,48 +2119,51 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="L12">
+      <c r="K12" s="2">
+        <v>2896</v>
+      </c>
+      <c r="M12">
+        <f>M11+E12</f>
+        <v>3000</v>
+      </c>
+      <c r="N12">
+        <f>N11+F12</f>
+        <v>3000</v>
+      </c>
+      <c r="O12">
+        <f>O11+G12</f>
+        <v>29322</v>
+      </c>
+      <c r="P12">
+        <f>P11+H12</f>
+        <v>1493</v>
+      </c>
+      <c r="Q12">
+        <f>Q11+I12</f>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f>R11+J12</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="1"/>
-        <v>29322</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="1"/>
-        <v>1493</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S12">
+        <v>31</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="4"/>
+        <v>23085</v>
+      </c>
+      <c r="W12">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="5"/>
-        <v>23085</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="3"/>
         <v>23285</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>32</v>
       </c>
@@ -2166,48 +2185,51 @@
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="L13">
+      <c r="K13" s="2">
+        <v>622</v>
+      </c>
+      <c r="M13">
+        <f>M12+E13</f>
+        <v>3000</v>
+      </c>
+      <c r="N13">
+        <f>N12+F13</f>
+        <v>3394</v>
+      </c>
+      <c r="O13">
+        <f>O12+G13</f>
+        <v>33322</v>
+      </c>
+      <c r="P13">
+        <f>P12+H13</f>
+        <v>8813</v>
+      </c>
+      <c r="Q13">
+        <f>Q12+I13</f>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f>R12+J13</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>3394</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>33322</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="1"/>
-        <v>8813</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S13">
+        <v>32</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="4"/>
+        <v>30815</v>
+      </c>
+      <c r="W13">
         <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="4"/>
-        <v>2000</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="5"/>
-        <v>30815</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="3"/>
         <v>32815</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>33</v>
       </c>
@@ -2225,48 +2247,49 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="L14">
+      <c r="K14" s="2"/>
+      <c r="M14">
+        <f>M13+E14</f>
+        <v>3000</v>
+      </c>
+      <c r="N14">
+        <f>N13+F14</f>
+        <v>3394</v>
+      </c>
+      <c r="O14">
+        <f>O13+G14</f>
+        <v>33322</v>
+      </c>
+      <c r="P14">
+        <f>P13+H14</f>
+        <v>11361</v>
+      </c>
+      <c r="Q14">
+        <f>Q13+I14</f>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f>R13+J14</f>
+        <v>0</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>3394</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>33322</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="1"/>
-        <v>11361</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S14">
+        <v>33</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="4"/>
+        <v>42135</v>
+      </c>
+      <c r="W14">
         <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="4"/>
-        <v>6000</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="5"/>
-        <v>42135</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="3"/>
         <v>48135</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>34</v>
       </c>
@@ -2282,48 +2305,49 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="L15">
+      <c r="K15" s="2"/>
+      <c r="M15">
+        <f>M14+E15</f>
+        <v>3000</v>
+      </c>
+      <c r="N15">
+        <f>N14+F15</f>
+        <v>3394</v>
+      </c>
+      <c r="O15">
+        <f>O14+G15</f>
+        <v>33322</v>
+      </c>
+      <c r="P15">
+        <f>P14+H15</f>
+        <v>11361</v>
+      </c>
+      <c r="Q15">
+        <f>Q14+I15</f>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f>R14+J15</f>
+        <v>0</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
-        <v>3394</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="1"/>
-        <v>33322</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="1"/>
-        <v>11361</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S15">
+        <v>34</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="3"/>
+        <v>6394</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="4"/>
+        <v>44683</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="4"/>
-        <v>6394</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="5"/>
-        <v>44683</v>
-      </c>
-      <c r="V15">
-        <f t="shared" si="3"/>
         <v>51077</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>35</v>
       </c>
@@ -2339,48 +2363,49 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="L16">
+      <c r="K16" s="2"/>
+      <c r="M16">
+        <f>M15+E16</f>
+        <v>3000</v>
+      </c>
+      <c r="N16">
+        <f>N15+F16</f>
+        <v>3394</v>
+      </c>
+      <c r="O16">
+        <f>O15+G16</f>
+        <v>33322</v>
+      </c>
+      <c r="P16">
+        <f>P15+H16</f>
+        <v>11361</v>
+      </c>
+      <c r="Q16">
+        <f>Q15+I16</f>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f>R15+J16</f>
+        <v>0</v>
+      </c>
+      <c r="T16">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="1"/>
-        <v>3394</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="1"/>
-        <v>33322</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="1"/>
-        <v>11361</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S16">
+        <v>35</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="3"/>
+        <v>6394</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="4"/>
+        <v>44683</v>
+      </c>
+      <c r="W16">
         <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="4"/>
-        <v>6394</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="5"/>
-        <v>44683</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="3"/>
         <v>51077</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>36</v>
       </c>
@@ -2396,79 +2421,81 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="L17">
+      <c r="K17" s="2"/>
+      <c r="M17">
+        <f>M16+E17</f>
+        <v>3000</v>
+      </c>
+      <c r="N17">
+        <f>N16+F17</f>
+        <v>3394</v>
+      </c>
+      <c r="O17">
+        <f>O16+G17</f>
+        <v>33322</v>
+      </c>
+      <c r="P17">
+        <f>P16+H17</f>
+        <v>11361</v>
+      </c>
+      <c r="Q17">
+        <f>Q16+I17</f>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>R16+J17</f>
+        <v>0</v>
+      </c>
+      <c r="T17">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="1"/>
-        <v>3394</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
-        <v>33322</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="1"/>
-        <v>11361</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S17">
+        <v>36</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="3"/>
+        <v>6394</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="4"/>
+        <v>44683</v>
+      </c>
+      <c r="W17">
         <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="4"/>
-        <v>6394</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="5"/>
-        <v>44683</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="3"/>
         <v>51077</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" ref="E18:J18" si="6">SUM(E7:E17)</f>
+        <f t="shared" ref="E18:J18" si="5">SUM(E7:E17)</f>
         <v>3000</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3394</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>33315</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11361</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="E3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2482,9 +2509,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2495,7 +2522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>45452</v>
       </c>
@@ -2504,11 +2531,11 @@
         <v>24</v>
       </c>
       <c r="C2" s="10">
-        <f>VLOOKUP('inriver catch'!B2,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B2,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>45453</v>
       </c>
@@ -2517,11 +2544,11 @@
         <v>24</v>
       </c>
       <c r="C3" s="10">
-        <f>VLOOKUP('inriver catch'!B3,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B3,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>45454</v>
       </c>
@@ -2530,11 +2557,11 @@
         <v>24</v>
       </c>
       <c r="C4" s="10">
-        <f>VLOOKUP('inriver catch'!B4,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B4,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>45455</v>
       </c>
@@ -2543,11 +2570,11 @@
         <v>24</v>
       </c>
       <c r="C5" s="10">
-        <f>VLOOKUP('inriver catch'!B5,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B5,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>45456</v>
       </c>
@@ -2556,11 +2583,11 @@
         <v>24</v>
       </c>
       <c r="C6" s="10">
-        <f>VLOOKUP('inriver catch'!B6,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B6,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>45457</v>
       </c>
@@ -2569,11 +2596,11 @@
         <v>24</v>
       </c>
       <c r="C7" s="10">
-        <f>VLOOKUP('inriver catch'!B7,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B7,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>45458</v>
       </c>
@@ -2582,11 +2609,11 @@
         <v>24</v>
       </c>
       <c r="C8" s="10">
-        <f>VLOOKUP('inriver catch'!B8,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B8,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>45459</v>
       </c>
@@ -2595,11 +2622,11 @@
         <v>25</v>
       </c>
       <c r="C9" s="10">
-        <f>VLOOKUP('inriver catch'!B9,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B9,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>45460</v>
       </c>
@@ -2608,11 +2635,11 @@
         <v>25</v>
       </c>
       <c r="C10" s="10">
-        <f>VLOOKUP('inriver catch'!B10,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B10,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>45461</v>
       </c>
@@ -2621,11 +2648,11 @@
         <v>25</v>
       </c>
       <c r="C11" s="10">
-        <f>VLOOKUP('inriver catch'!B11,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B11,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>45462</v>
       </c>
@@ -2634,11 +2661,11 @@
         <v>25</v>
       </c>
       <c r="C12" s="10">
-        <f>VLOOKUP('inriver catch'!B12,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B12,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>45463</v>
       </c>
@@ -2647,11 +2674,11 @@
         <v>25</v>
       </c>
       <c r="C13" s="10">
-        <f>VLOOKUP('inriver catch'!B13,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B13,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>45464</v>
       </c>
@@ -2660,11 +2687,11 @@
         <v>25</v>
       </c>
       <c r="C14" s="10">
-        <f>VLOOKUP('inriver catch'!B14,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B14,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>45465</v>
       </c>
@@ -2673,11 +2700,11 @@
         <v>25</v>
       </c>
       <c r="C15" s="10">
-        <f>VLOOKUP('inriver catch'!B15,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+        <f>VLOOKUP('inriver catch'!B15,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>45466</v>
       </c>
@@ -2686,11 +2713,11 @@
         <v>26</v>
       </c>
       <c r="C16" s="10">
-        <f>VLOOKUP('inriver catch'!B16,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B16,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>45467</v>
       </c>
@@ -2699,11 +2726,11 @@
         <v>26</v>
       </c>
       <c r="C17" s="10">
-        <f>VLOOKUP('inriver catch'!B17,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B17,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>45468</v>
       </c>
@@ -2712,11 +2739,11 @@
         <v>26</v>
       </c>
       <c r="C18" s="10">
-        <f>VLOOKUP('inriver catch'!B18,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B18,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>45469</v>
       </c>
@@ -2725,11 +2752,11 @@
         <v>26</v>
       </c>
       <c r="C19" s="10">
-        <f>VLOOKUP('inriver catch'!B19,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B19,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>45470</v>
       </c>
@@ -2738,11 +2765,11 @@
         <v>26</v>
       </c>
       <c r="C20" s="10">
-        <f>VLOOKUP('inriver catch'!B20,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B20,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>45471</v>
       </c>
@@ -2751,11 +2778,11 @@
         <v>26</v>
       </c>
       <c r="C21" s="10">
-        <f>VLOOKUP('inriver catch'!B21,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B21,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>45472</v>
       </c>
@@ -2764,11 +2791,11 @@
         <v>26</v>
       </c>
       <c r="C22" s="10">
-        <f>VLOOKUP('inriver catch'!B22,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B22,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>45473</v>
       </c>
@@ -2777,11 +2804,11 @@
         <v>27</v>
       </c>
       <c r="C23" s="10">
-        <f>VLOOKUP('inriver catch'!B23,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B23,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>45474</v>
       </c>
@@ -2790,11 +2817,11 @@
         <v>27</v>
       </c>
       <c r="C24" s="10">
-        <f>VLOOKUP('inriver catch'!B24,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B24,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>45475</v>
       </c>
@@ -2803,11 +2830,11 @@
         <v>27</v>
       </c>
       <c r="C25" s="10">
-        <f>VLOOKUP('inriver catch'!B25,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B25,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>45476</v>
       </c>
@@ -2816,11 +2843,11 @@
         <v>27</v>
       </c>
       <c r="C26" s="10">
-        <f>VLOOKUP('inriver catch'!B26,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B26,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>45477</v>
       </c>
@@ -2829,11 +2856,11 @@
         <v>27</v>
       </c>
       <c r="C27" s="10">
-        <f>VLOOKUP('inriver catch'!B27,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B27,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>45478</v>
       </c>
@@ -2842,11 +2869,11 @@
         <v>27</v>
       </c>
       <c r="C28" s="10">
-        <f>VLOOKUP('inriver catch'!B28,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B28,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>45479</v>
       </c>
@@ -2855,11 +2882,11 @@
         <v>27</v>
       </c>
       <c r="C29" s="10">
-        <f>VLOOKUP('inriver catch'!B29,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B29,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>45480</v>
       </c>
@@ -2868,11 +2895,11 @@
         <v>28</v>
       </c>
       <c r="C30" s="10">
-        <f>VLOOKUP('inriver catch'!B30,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B30,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>45481</v>
       </c>
@@ -2881,11 +2908,11 @@
         <v>28</v>
       </c>
       <c r="C31" s="10">
-        <f>VLOOKUP('inriver catch'!B31,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B31,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>45482</v>
       </c>
@@ -2894,11 +2921,11 @@
         <v>28</v>
       </c>
       <c r="C32" s="10">
-        <f>VLOOKUP('inriver catch'!B32,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B32,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>45483</v>
       </c>
@@ -2907,11 +2934,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="10">
-        <f>VLOOKUP('inriver catch'!B33,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B33,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>45484</v>
       </c>
@@ -2920,11 +2947,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="10">
-        <f>VLOOKUP('inriver catch'!B34,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B34,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>45485</v>
       </c>
@@ -2933,11 +2960,11 @@
         <v>28</v>
       </c>
       <c r="C35" s="10">
-        <f>VLOOKUP('inriver catch'!B35,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B35,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>45486</v>
       </c>
@@ -2946,11 +2973,11 @@
         <v>28</v>
       </c>
       <c r="C36" s="10">
-        <f>VLOOKUP('inriver catch'!B36,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B36,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>2418</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>45487</v>
       </c>
@@ -2959,11 +2986,11 @@
         <v>29</v>
       </c>
       <c r="C37" s="10">
-        <f>VLOOKUP('inriver catch'!B37,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B37,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>45488</v>
       </c>
@@ -2972,11 +2999,11 @@
         <v>29</v>
       </c>
       <c r="C38" s="10">
-        <f>VLOOKUP('inriver catch'!B38,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B38,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>45489</v>
       </c>
@@ -2985,11 +3012,11 @@
         <v>29</v>
       </c>
       <c r="C39" s="10">
-        <f>VLOOKUP('inriver catch'!B39,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B39,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>45490</v>
       </c>
@@ -2998,11 +3025,11 @@
         <v>29</v>
       </c>
       <c r="C40" s="10">
-        <f>VLOOKUP('inriver catch'!B40,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B40,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>45491</v>
       </c>
@@ -3011,11 +3038,11 @@
         <v>29</v>
       </c>
       <c r="C41" s="10">
-        <f>VLOOKUP('inriver catch'!B41,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B41,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>45492</v>
       </c>
@@ -3024,11 +3051,11 @@
         <v>29</v>
       </c>
       <c r="C42" s="10">
-        <f>VLOOKUP('inriver catch'!B42,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B42,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>45493</v>
       </c>
@@ -3037,11 +3064,11 @@
         <v>29</v>
       </c>
       <c r="C43" s="10">
-        <f>VLOOKUP('inriver catch'!B43,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B43,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>6304</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>45494</v>
       </c>
@@ -3050,11 +3077,11 @@
         <v>30</v>
       </c>
       <c r="C44" s="10">
-        <f>VLOOKUP('inriver catch'!B44,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B44,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>45495</v>
       </c>
@@ -3063,11 +3090,11 @@
         <v>30</v>
       </c>
       <c r="C45" s="10">
-        <f>VLOOKUP('inriver catch'!B45,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B45,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>45496</v>
       </c>
@@ -3076,11 +3103,11 @@
         <v>30</v>
       </c>
       <c r="C46" s="10">
-        <f>VLOOKUP('inriver catch'!B46,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B46,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>45497</v>
       </c>
@@ -3089,11 +3116,11 @@
         <v>30</v>
       </c>
       <c r="C47" s="10">
-        <f>VLOOKUP('inriver catch'!B47,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B47,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>45498</v>
       </c>
@@ -3102,11 +3129,11 @@
         <v>30</v>
       </c>
       <c r="C48" s="10">
-        <f>VLOOKUP('inriver catch'!B48,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B48,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>45499</v>
       </c>
@@ -3115,11 +3142,11 @@
         <v>30</v>
       </c>
       <c r="C49" s="10">
-        <f>VLOOKUP('inriver catch'!B49,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B49,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>45500</v>
       </c>
@@ -3128,11 +3155,11 @@
         <v>30</v>
       </c>
       <c r="C50" s="10">
-        <f>VLOOKUP('inriver catch'!B50,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B50,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>14368</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>45501</v>
       </c>
@@ -3141,11 +3168,11 @@
         <v>31</v>
       </c>
       <c r="C51" s="10">
-        <f>VLOOKUP('inriver catch'!B51,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B51,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>45502</v>
       </c>
@@ -3154,11 +3181,11 @@
         <v>31</v>
       </c>
       <c r="C52" s="10">
-        <f>VLOOKUP('inriver catch'!B52,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B52,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>45503</v>
       </c>
@@ -3167,11 +3194,11 @@
         <v>31</v>
       </c>
       <c r="C53" s="10">
-        <f>VLOOKUP('inriver catch'!B53,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B53,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>45504</v>
       </c>
@@ -3180,11 +3207,11 @@
         <v>31</v>
       </c>
       <c r="C54" s="10">
-        <f>VLOOKUP('inriver catch'!B54,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B54,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
         <v>45505</v>
       </c>
@@ -3193,11 +3220,11 @@
         <v>31</v>
       </c>
       <c r="C55" s="10">
-        <f>VLOOKUP('inriver catch'!B55,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B55,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>45506</v>
       </c>
@@ -3206,11 +3233,11 @@
         <v>31</v>
       </c>
       <c r="C56" s="10">
-        <f>VLOOKUP('inriver catch'!B56,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B56,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>45507</v>
       </c>
@@ -3219,11 +3246,11 @@
         <v>31</v>
       </c>
       <c r="C57" s="10">
-        <f>VLOOKUP('inriver catch'!B57,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B57,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>23285</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>45508</v>
       </c>
@@ -3232,11 +3259,11 @@
         <v>32</v>
       </c>
       <c r="C58" s="10">
-        <f>VLOOKUP('inriver catch'!B58,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B58,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>45509</v>
       </c>
@@ -3245,11 +3272,11 @@
         <v>32</v>
       </c>
       <c r="C59" s="10">
-        <f>VLOOKUP('inriver catch'!B59,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B59,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>45510</v>
       </c>
@@ -3258,11 +3285,11 @@
         <v>32</v>
       </c>
       <c r="C60" s="10">
-        <f>VLOOKUP('inriver catch'!B60,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B60,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>45511</v>
       </c>
@@ -3271,11 +3298,11 @@
         <v>32</v>
       </c>
       <c r="C61" s="10">
-        <f>VLOOKUP('inriver catch'!B61,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B61,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>45512</v>
       </c>
@@ -3284,11 +3311,11 @@
         <v>32</v>
       </c>
       <c r="C62" s="10">
-        <f>VLOOKUP('inriver catch'!B62,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B62,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>45513</v>
       </c>
@@ -3297,11 +3324,11 @@
         <v>32</v>
       </c>
       <c r="C63" s="10">
-        <f>VLOOKUP('inriver catch'!B63,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B63,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
         <v>45514</v>
       </c>
@@ -3310,11 +3337,11 @@
         <v>32</v>
       </c>
       <c r="C64" s="10">
-        <f>VLOOKUP('inriver catch'!B64,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B64,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>32815</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>45515</v>
       </c>
@@ -3323,11 +3350,11 @@
         <v>33</v>
       </c>
       <c r="C65" s="10">
-        <f>VLOOKUP('inriver catch'!B65,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B65,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>48135</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>45516</v>
       </c>
@@ -3336,11 +3363,11 @@
         <v>33</v>
       </c>
       <c r="C66" s="10">
-        <f>VLOOKUP('inriver catch'!B66,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B66,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>48135</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>45517</v>
       </c>
@@ -3349,11 +3376,11 @@
         <v>33</v>
       </c>
       <c r="C67" s="10">
-        <f>VLOOKUP('inriver catch'!B67,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B67,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>48135</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
         <v>45518</v>
       </c>
@@ -3362,11 +3389,11 @@
         <v>33</v>
       </c>
       <c r="C68" s="10">
-        <f>VLOOKUP('inriver catch'!B68,'Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
+        <f>VLOOKUP('inriver catch'!B68,'Sockeye FSC and Demo'!$T$5:$W$17,4,FALSE)</f>
         <v>48135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
         <v>45519</v>
       </c>
@@ -3376,7 +3403,7 @@
       </c>
       <c r="C69" s="10"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
         <v>45520</v>
       </c>
@@ -3386,7 +3413,7 @@
       </c>
       <c r="C70" s="10"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="11">
         <v>45521</v>
       </c>
@@ -3396,7 +3423,7 @@
       </c>
       <c r="C71" s="10"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>45522</v>
       </c>
@@ -3406,7 +3433,7 @@
       </c>
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>45523</v>
       </c>
@@ -3416,7 +3443,7 @@
       </c>
       <c r="C73" s="10"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>45524</v>
       </c>
@@ -3426,7 +3453,7 @@
       </c>
       <c r="C74" s="10"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>45525</v>
       </c>
@@ -3436,7 +3463,7 @@
       </c>
       <c r="C75" s="10"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>45526</v>
       </c>
@@ -3446,7 +3473,7 @@
       </c>
       <c r="C76" s="10"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
         <v>45527</v>
       </c>
@@ -3456,7 +3483,7 @@
       </c>
       <c r="C77" s="10"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
         <v>45528</v>
       </c>
@@ -3466,7 +3493,7 @@
       </c>
       <c r="C78" s="10"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="11">
         <v>45529</v>
       </c>
@@ -3476,7 +3503,7 @@
       </c>
       <c r="C79" s="10"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
         <v>45530</v>
       </c>
@@ -3486,7 +3513,7 @@
       </c>
       <c r="C80" s="10"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
         <v>45531</v>
       </c>
@@ -3496,7 +3523,7 @@
       </c>
       <c r="C81" s="10"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
         <v>45532</v>
       </c>
@@ -3506,7 +3533,7 @@
       </c>
       <c r="C82" s="10"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
         <v>45533</v>
       </c>
@@ -3516,7 +3543,7 @@
       </c>
       <c r="C83" s="10"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
         <v>45534</v>
       </c>
@@ -3526,7 +3553,7 @@
       </c>
       <c r="C84" s="10"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
         <v>45535</v>
       </c>
@@ -3536,7 +3563,7 @@
       </c>
       <c r="C85" s="10"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
         <v>45536</v>
       </c>
@@ -3546,7 +3573,7 @@
       </c>
       <c r="C86" s="10"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
         <v>45537</v>
       </c>
@@ -3556,7 +3583,7 @@
       </c>
       <c r="C87" s="10"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="11">
         <v>45538</v>
       </c>
@@ -3566,7 +3593,7 @@
       </c>
       <c r="C88" s="10"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
         <v>45539</v>
       </c>
@@ -3576,7 +3603,7 @@
       </c>
       <c r="C89" s="10"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="11">
         <v>45540</v>
       </c>
@@ -3586,7 +3613,7 @@
       </c>
       <c r="C90" s="10"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
         <v>45541</v>
       </c>
@@ -3596,7 +3623,7 @@
       </c>
       <c r="C91" s="10"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="11">
         <v>45542</v>
       </c>
@@ -3613,18 +3640,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A7F00F-86F9-7B42-9119-B394F847541D}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3644,7 +3671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>45490</v>
       </c>
@@ -3658,7 +3685,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>45490</v>
       </c>
@@ -3672,7 +3699,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>45497</v>
       </c>
@@ -3686,7 +3713,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>45501</v>
       </c>
@@ -3700,7 +3727,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>45501</v>
       </c>
@@ -3714,7 +3741,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>45505</v>
       </c>
@@ -3728,7 +3755,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>45506</v>
       </c>
@@ -3742,7 +3769,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>45506</v>
       </c>
@@ -3756,7 +3783,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>45508</v>
       </c>
@@ -3770,7 +3797,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>45509</v>
       </c>
@@ -3784,7 +3811,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>45509</v>
       </c>
@@ -3798,7 +3825,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>45510</v>
       </c>
@@ -3812,7 +3839,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>45510</v>
       </c>
@@ -3826,7 +3853,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>45510</v>
       </c>
@@ -3840,7 +3867,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>45511</v>
       </c>
@@ -3854,7 +3881,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>45511</v>
       </c>
@@ -3868,7 +3895,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>45512</v>
       </c>
@@ -3882,7 +3909,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>45513</v>
       </c>
@@ -3896,7 +3923,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>45514</v>
       </c>
@@ -3910,7 +3937,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>45515</v>
       </c>
@@ -3924,7 +3951,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>45515</v>
       </c>
@@ -3938,7 +3965,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>45516</v>
       </c>
@@ -3952,7 +3979,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>45517</v>
       </c>
@@ -3966,7 +3993,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>45518</v>
       </c>
@@ -3980,7 +4007,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>45519</v>
       </c>
@@ -3994,7 +4021,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>45520</v>
       </c>
@@ -4008,7 +4035,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>45521</v>
       </c>
@@ -4022,7 +4049,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>45522</v>
       </c>
@@ -4036,7 +4063,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>45523</v>
       </c>
@@ -4048,6 +4075,146 @@
       </c>
       <c r="D30">
         <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>45504</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="11">
+        <v>45505</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="11">
+        <v>45506</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="11">
+        <v>45508</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="11">
+        <v>45509</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="11">
+        <v>45510</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="11">
+        <v>45511</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="11">
+        <v>45512</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="11">
+        <v>45513</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="11">
+        <v>45514</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add LBN demo catch numbers
</commit_message>
<xml_diff>
--- a/data/FNs catch 2024.xlsx
+++ b/data/FNs catch 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773DDB40-28A5-8647-B660-428C85447036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC7A99-C134-9F47-B316-4519F49B9575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="500" windowWidth="27820" windowHeight="17500" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sockeye FSC and Demo" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="32">
   <si>
     <t>In-River Skeena FSC Catch Numbers - DO NOT SHARE BEYOND SFNTC</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Metlakatla</t>
+  </si>
+  <si>
+    <t>Lake Babine</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1558,7 @@
   <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1749,31 +1752,31 @@
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
       <c r="M6">
-        <f>M5+E6</f>
+        <f t="shared" ref="M6:M17" si="1">M5+E6</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>N5+F6</f>
+        <f t="shared" ref="N6:N17" si="2">N5+F6</f>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>O5+G6</f>
+        <f t="shared" ref="O6:O17" si="3">O5+G6</f>
         <v>7</v>
       </c>
       <c r="P6">
-        <f>P5+H6</f>
+        <f t="shared" ref="P6:P17" si="4">P5+H6</f>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>Q5+I6</f>
+        <f t="shared" ref="Q6:Q17" si="5">Q5+I6</f>
         <v>0</v>
       </c>
       <c r="R6">
-        <f>R5+J6</f>
+        <f t="shared" ref="R6:R17" si="6">R5+J6</f>
         <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:T17" si="1">A6</f>
+        <f t="shared" ref="T6:T17" si="7">A6</f>
         <v>25</v>
       </c>
       <c r="U6">
@@ -1783,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" ref="W6:W17" si="2">SUM(U6:V6)</f>
+        <f t="shared" ref="W6:W17" si="8">SUM(U6:V6)</f>
         <v>0</v>
       </c>
     </row>
@@ -1807,43 +1810,43 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="M7">
-        <f>M6+E7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>N6+F7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O7">
-        <f>O6+G7</f>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="P7">
-        <f>P6+H7</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>Q6+I7</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>R6+J7</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="U7">
-        <f t="shared" ref="U7:U17" si="3">SUM(M5+N5)</f>
+        <f t="shared" ref="U7:U17" si="9">SUM(M5+N5)</f>
         <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" ref="V7:V17" si="4">SUM(O6+P6)</f>
+        <f t="shared" ref="V7:V17" si="10">SUM(O6+P6)</f>
         <v>7</v>
       </c>
       <c r="W7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
@@ -1867,43 +1870,43 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="M8">
-        <f>M7+E8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>N7+F8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>O7+G8</f>
+        <f t="shared" si="3"/>
         <v>2418</v>
       </c>
       <c r="P8">
-        <f>P7+H8</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>Q7+I8</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>R7+J8</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="U8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>86</v>
       </c>
       <c r="W8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>86</v>
       </c>
     </row>
@@ -1927,43 +1930,43 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="M9">
-        <f>M8+E9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>N8+F9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>O8+G9</f>
+        <f t="shared" si="3"/>
         <v>6304</v>
       </c>
       <c r="P9">
-        <f>P8+H9</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>Q8+I9</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>R8+J9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="U9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2418</v>
       </c>
       <c r="W9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2418</v>
       </c>
     </row>
@@ -1991,43 +1994,43 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="M10">
-        <f>M9+E10</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="N10">
-        <f>N9+F10</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="O10">
-        <f>O9+G10</f>
+        <f t="shared" si="3"/>
         <v>14368</v>
       </c>
       <c r="P10">
-        <f>P9+H10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>Q9+I10</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>R9+J10</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="U10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>6304</v>
       </c>
       <c r="W10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6304</v>
       </c>
     </row>
@@ -2055,43 +2058,43 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="M11">
-        <f>M10+E11</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="N11">
-        <f>N10+F11</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="O11">
-        <f>O10+G11</f>
+        <f t="shared" si="3"/>
         <v>23085</v>
       </c>
       <c r="P11">
-        <f>P10+H11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>Q10+I11</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>R10+J11</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="U11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>14368</v>
       </c>
       <c r="W11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>14368</v>
       </c>
     </row>
@@ -2123,43 +2126,43 @@
         <v>2896</v>
       </c>
       <c r="M12">
-        <f>M11+E12</f>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
       <c r="N12">
-        <f>N11+F12</f>
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="O12">
-        <f>O11+G12</f>
+        <f t="shared" si="3"/>
         <v>29322</v>
       </c>
       <c r="P12">
-        <f>P11+H12</f>
+        <f t="shared" si="4"/>
         <v>1493</v>
       </c>
       <c r="Q12">
-        <f>Q11+I12</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>R11+J12</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="U12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>200</v>
       </c>
       <c r="V12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>23085</v>
       </c>
       <c r="W12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>23285</v>
       </c>
     </row>
@@ -2189,43 +2192,43 @@
         <v>622</v>
       </c>
       <c r="M13">
-        <f>M12+E13</f>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
       <c r="N13">
-        <f>N12+F13</f>
+        <f t="shared" si="2"/>
         <v>3394</v>
       </c>
       <c r="O13">
-        <f>O12+G13</f>
+        <f t="shared" si="3"/>
         <v>33322</v>
       </c>
       <c r="P13">
-        <f>P12+H13</f>
+        <f t="shared" si="4"/>
         <v>8813</v>
       </c>
       <c r="Q13">
-        <f>Q12+I13</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>R12+J13</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="U13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2000</v>
       </c>
       <c r="V13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>30815</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>32815</v>
       </c>
     </row>
@@ -2249,43 +2252,43 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="M14">
-        <f>M13+E14</f>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
       <c r="N14">
-        <f>N13+F14</f>
+        <f t="shared" si="2"/>
         <v>3394</v>
       </c>
       <c r="O14">
-        <f>O13+G14</f>
+        <f t="shared" si="3"/>
         <v>33322</v>
       </c>
       <c r="P14">
-        <f>P13+H14</f>
+        <f t="shared" si="4"/>
         <v>11361</v>
       </c>
       <c r="Q14">
-        <f>Q13+I14</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>R13+J14</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="U14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6000</v>
       </c>
       <c r="V14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>42135</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>48135</v>
       </c>
     </row>
@@ -2307,43 +2310,43 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15">
-        <f>M14+E15</f>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
       <c r="N15">
-        <f>N14+F15</f>
+        <f t="shared" si="2"/>
         <v>3394</v>
       </c>
       <c r="O15">
-        <f>O14+G15</f>
+        <f t="shared" si="3"/>
         <v>33322</v>
       </c>
       <c r="P15">
-        <f>P14+H15</f>
+        <f t="shared" si="4"/>
         <v>11361</v>
       </c>
       <c r="Q15">
-        <f>Q14+I15</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>R14+J15</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6394</v>
       </c>
       <c r="V15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>44683</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>51077</v>
       </c>
     </row>
@@ -2362,46 +2365,48 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2">
+        <v>34030</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="M16">
-        <f>M15+E16</f>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
       <c r="N16">
-        <f>N15+F16</f>
+        <f t="shared" si="2"/>
         <v>3394</v>
       </c>
       <c r="O16">
-        <f>O15+G16</f>
+        <f t="shared" si="3"/>
         <v>33322</v>
       </c>
       <c r="P16">
-        <f>P15+H16</f>
+        <f t="shared" si="4"/>
         <v>11361</v>
       </c>
       <c r="Q16">
-        <f>Q15+I16</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>R15+J16</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>34030</v>
       </c>
       <c r="T16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="U16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6394</v>
       </c>
       <c r="V16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>44683</v>
       </c>
       <c r="W16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>51077</v>
       </c>
     </row>
@@ -2423,43 +2428,43 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17">
-        <f>M16+E17</f>
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
       <c r="N17">
-        <f>N16+F17</f>
+        <f t="shared" si="2"/>
         <v>3394</v>
       </c>
       <c r="O17">
-        <f>O16+G17</f>
+        <f t="shared" si="3"/>
         <v>33322</v>
       </c>
       <c r="P17">
-        <f>P16+H17</f>
+        <f t="shared" si="4"/>
         <v>11361</v>
       </c>
       <c r="Q17">
-        <f>Q16+I17</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R17">
-        <f>R16+J17</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>34030</v>
       </c>
       <c r="T17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="U17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6394</v>
       </c>
       <c r="V17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>44683</v>
       </c>
       <c r="W17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>51077</v>
       </c>
     </row>
@@ -2468,28 +2473,28 @@
         <v>17</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" ref="E18:J18" si="5">SUM(E7:E17)</f>
+        <f t="shared" ref="E18:J18" si="11">SUM(E7:E17)</f>
         <v>3000</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>3394</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>33315</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>11361</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>34030</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -3640,10 +3645,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A7F00F-86F9-7B42-9119-B394F847541D}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4217,6 +4222,90 @@
         <v>41</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="11">
+        <v>45529</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="11">
+        <v>45531</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="11">
+        <v>45532</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43">
+        <v>6510</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="11">
+        <v>45533</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44">
+        <v>11130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="11">
+        <v>45534</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="11">
+        <v>45535</v>
+      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46">
+        <v>8200</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
     <sortCondition ref="A2:A23"/>

</xml_diff>